<commit_message>
Half of part1: Exercise 1.1-1.6
</commit_message>
<xml_diff>
--- a/hour diary.xlsx
+++ b/hour diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yliopisto_local\devops_with_docker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B0DA29-08BE-4077-8FEE-FBE831366A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6148696A-308B-460A-B671-52124525769C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{41530EE6-227F-4373-A0DE-86C5D2F2675E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41530EE6-227F-4373-A0DE-86C5D2F2675E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,24 +34,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>pvm</t>
   </si>
   <si>
-    <t>aika</t>
-  </si>
-  <si>
-    <t>osa</t>
-  </si>
-  <si>
-    <t>yht</t>
-  </si>
-  <si>
-    <t>kommentti</t>
-  </si>
-  <si>
-    <t>osa 0 ja 1 ja tehtäväpalautus materiaalien luku</t>
+    <t>time (min)</t>
+  </si>
+  <si>
+    <t>part</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>time (hour)</t>
+  </si>
+  <si>
+    <t>read more part 1 and do ex 1.1 and 1.2</t>
+  </si>
+  <si>
+    <t>ex 1.3 and 1.4 and respective material</t>
+  </si>
+  <si>
+    <t>ex 1.5 and 1.6 and respective material</t>
+  </si>
+  <si>
+    <t>read material of parts 0 and 1 and exercise guide and install stuff</t>
   </si>
 </sst>
 </file>
@@ -403,15 +412,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24189A99-566E-475A-B291-BDDA587D2298}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="57.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -425,10 +436,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -442,11 +453,53 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <f>SUM(B2:B38)/60</f>
-        <v>2</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>210824</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>210831</v>
+      </c>
+      <c r="B4">
+        <v>80</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>210908</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Exercises 1.7 and 1.8
</commit_message>
<xml_diff>
--- a/hour diary.xlsx
+++ b/hour diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yliopisto_local\devops_with_docker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6148696A-308B-460A-B671-52124525769C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8C8EB9-A5E6-45AF-9CA4-D60878436545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41530EE6-227F-4373-A0DE-86C5D2F2675E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>pvm</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>read material of parts 0 and 1 and exercise guide and install stuff</t>
+  </si>
+  <si>
+    <t>ex 1.7 and material</t>
+  </si>
+  <si>
+    <t>ex 1.8</t>
   </si>
 </sst>
 </file>
@@ -412,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24189A99-566E-475A-B291-BDDA587D2298}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +463,7 @@
       </c>
       <c r="G2">
         <f>SUM(B2:B38)/60</f>
-        <v>5</v>
+        <v>6.333333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -500,6 +506,34 @@
       </c>
       <c r="D5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>210909</v>
+      </c>
+      <c r="B6">
+        <v>60</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>210910</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add exercises 1.10 and 1.11
</commit_message>
<xml_diff>
--- a/hour diary.xlsx
+++ b/hour diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yliopisto_local\devops_with_docker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8C8EB9-A5E6-45AF-9CA4-D60878436545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39D10B8-D3D6-4493-ABE9-82561C7F0F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41530EE6-227F-4373-A0DE-86C5D2F2675E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>pvm</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>ex 1.8</t>
+  </si>
+  <si>
+    <t>ex 1.9-1.11 and material</t>
   </si>
 </sst>
 </file>
@@ -418,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24189A99-566E-475A-B291-BDDA587D2298}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +466,7 @@
       </c>
       <c r="G2">
         <f>SUM(B2:B38)/60</f>
-        <v>6.333333333333333</v>
+        <v>8.3333333333333339</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -534,6 +537,20 @@
       </c>
       <c r="D7" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>210912</v>
+      </c>
+      <c r="B8">
+        <v>120</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add exercise 1.12 and modify gitignore
</commit_message>
<xml_diff>
--- a/hour diary.xlsx
+++ b/hour diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yliopisto_local\devops_with_docker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39D10B8-D3D6-4493-ABE9-82561C7F0F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F72188-9706-49FA-B6C2-06E5CBDD334B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41530EE6-227F-4373-A0DE-86C5D2F2675E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>pvm</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>ex 1.9-1.11 and material</t>
+  </si>
+  <si>
+    <t>ex 1.12</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24189A99-566E-475A-B291-BDDA587D2298}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +469,7 @@
       </c>
       <c r="G2">
         <f>SUM(B2:B38)/60</f>
-        <v>8.3333333333333339</v>
+        <v>8.8333333333333339</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -551,6 +554,20 @@
       </c>
       <c r="D8" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>211001</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add url to 1.16
</commit_message>
<xml_diff>
--- a/hour diary.xlsx
+++ b/hour diary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yliopisto_local\devops_with_docker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F72188-9706-49FA-B6C2-06E5CBDD334B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63579905-62D9-4BDA-A8B1-2975A71D5505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41530EE6-227F-4373-A0DE-86C5D2F2675E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>pvm</t>
   </si>
@@ -72,7 +72,10 @@
     <t>ex 1.9-1.11 and material</t>
   </si>
   <si>
-    <t>ex 1.12</t>
+    <t>ex 1.12-1.13</t>
+  </si>
+  <si>
+    <t>ex 1.14 and 1.16</t>
   </si>
 </sst>
 </file>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24189A99-566E-475A-B291-BDDA587D2298}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +472,7 @@
       </c>
       <c r="G2">
         <f>SUM(B2:B38)/60</f>
-        <v>8.8333333333333339</v>
+        <v>10.666666666666666</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -561,13 +564,27 @@
         <v>211001</v>
       </c>
       <c r="B9">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>211030</v>
+      </c>
+      <c r="B10">
+        <v>90</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit diary to have parts as separate sheets
</commit_message>
<xml_diff>
--- a/hour diary.xlsx
+++ b/hour diary.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yliopisto_local\devops_with_docker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63579905-62D9-4BDA-A8B1-2975A71D5505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203CFD3D-102A-4E4B-B7D2-27B17357FDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41530EE6-227F-4373-A0DE-86C5D2F2675E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{41530EE6-227F-4373-A0DE-86C5D2F2675E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="part3" sheetId="4" r:id="rId1"/>
+    <sheet name="part2" sheetId="3" r:id="rId2"/>
+    <sheet name="part1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>pvm</t>
   </si>
@@ -42,9 +44,6 @@
     <t>time (min)</t>
   </si>
   <si>
-    <t>part</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -76,6 +75,9 @@
   </si>
   <si>
     <t>ex 1.14 and 1.16</t>
+  </si>
+  <si>
+    <t>Submit and edit diary</t>
   </si>
 </sst>
 </file>
@@ -426,21 +428,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24189A99-566E-475A-B291-BDDA587D2298}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E1B8B5-1972-4623-AC0C-36F617C50DC1}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="57.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,140 +452,201 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>SUM(B2:B38)/60</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B36FD07-54A7-4E39-9C13-88497F7DAE35}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>SUM(B2:B38)/60</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24189A99-566E-475A-B291-BDDA587D2298}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>210824</v>
       </c>
       <c r="B2">
         <v>120</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
         <f>SUM(B2:B38)/60</f>
-        <v>10.666666666666666</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10.833333333333334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>210824</v>
       </c>
       <c r="B3">
         <v>50</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>210831</v>
       </c>
       <c r="B4">
         <v>80</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>210908</v>
       </c>
       <c r="B5">
         <v>50</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>210909</v>
       </c>
       <c r="B6">
         <v>60</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>210910</v>
       </c>
       <c r="B7">
         <v>20</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>210912</v>
       </c>
       <c r="B8">
         <v>120</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>211001</v>
       </c>
       <c r="B9">
         <v>50</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>211030</v>
       </c>
       <c r="B10">
         <v>90</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>211101</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 2.5 and 2.6
</commit_message>
<xml_diff>
--- a/hour diary.xlsx
+++ b/hour diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yliopisto_local\devops_with_docker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFFCAFC-520C-4285-8517-932B14088B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB50283E-E6E6-4EE5-BA6E-DE62DDA0B95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{41530EE6-227F-4373-A0DE-86C5D2F2675E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>pvm</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>ex 2.2-2.4 and material</t>
+  </si>
+  <si>
+    <t>ex 2.5-2.6 and material</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B36FD07-54A7-4E39-9C13-88497F7DAE35}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +517,7 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B38)/60</f>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -526,6 +529,18 @@
       </c>
       <c r="C3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>211103</v>
+      </c>
+      <c r="B4">
+        <f>30+30</f>
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 2.7, 2.8, 2.9 which were done earlier
</commit_message>
<xml_diff>
--- a/hour diary.xlsx
+++ b/hour diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yliopisto_local\devops_with_docker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB50283E-E6E6-4EE5-BA6E-DE62DDA0B95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC3FD32-D6D7-4E62-B913-1B3E2C331B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{41530EE6-227F-4373-A0DE-86C5D2F2675E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>pvm</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>ex 2.5-2.6 and material</t>
+  </si>
+  <si>
+    <t>ex 2.7</t>
+  </si>
+  <si>
+    <t>ex 2.8 &amp; 2.9</t>
   </si>
 </sst>
 </file>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B36FD07-54A7-4E39-9C13-88497F7DAE35}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +523,7 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B38)/60</f>
-        <v>4.5</v>
+        <v>5.666666666666667</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -541,6 +547,29 @@
       </c>
       <c r="C4" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>211109</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>211117</v>
+      </c>
+      <c r="B6">
+        <f>30+10</f>
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add end of part2 to diary
</commit_message>
<xml_diff>
--- a/hour diary.xlsx
+++ b/hour diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yliopisto_local\devops_with_docker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC3FD32-D6D7-4E62-B913-1B3E2C331B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82A770B-F3C0-4FB9-9197-906FE29C38DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{41530EE6-227F-4373-A0DE-86C5D2F2675E}"/>
+    <workbookView xWindow="2895" yWindow="2460" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{41530EE6-227F-4373-A0DE-86C5D2F2675E}"/>
   </bookViews>
   <sheets>
     <sheet name="part3" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>pvm</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>ex 2.8 &amp; 2.9</t>
+  </si>
+  <si>
+    <t>Test 2.9 and do 2.10</t>
   </si>
 </sst>
 </file>
@@ -484,10 +487,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B36FD07-54A7-4E39-9C13-88497F7DAE35}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +526,7 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B38)/60</f>
-        <v>5.666666666666667</v>
+        <v>6.166666666666667</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -570,6 +573,17 @@
       </c>
       <c r="C6" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>211129</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>